<commit_message>
i442--pn eit2 suite update
</commit_message>
<xml_diff>
--- a/tmp_client/doc/TMP_EIT_suites/radiant/pn_20_project_navigator.xlsx
+++ b/tmp_client/doc/TMP_EIT_suites/radiant/pn_20_project_navigator.xlsx
@@ -1,16 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\qa\qausr\jwang1\project\TMP_EIT_suites\others\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\repository\tmp_client\doc\TMP_EIT_suites\radiant\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:81_{E67DCD3C-3BB6-41B2-A141-1682C6EE981B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="BBPw5sjxCCUVqKqDFh1VvlGl+6jBsyEv58ubpDIjFduKT4EttifNtZLgNn2j4jGi/bvDsFNRyO0+XWiClC3JHw==" workbookSaltValue="FQsz7bLsuDdqgfH6Nya7QA==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="6300" windowWidth="28830" windowHeight="6240"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="suite" sheetId="1" r:id="rId1"/>
@@ -25,18 +26,31 @@
     <definedName name="Z_7D13FC9B_B344_4E74_B7B7_44B6EA59DFDB_.wvu.FilterData" localSheetId="1" hidden="1">case!$A$2:$AD$2</definedName>
     <definedName name="Z_E811CF45_D5B3_4449_84AE_1514F9E9258F_.wvu.FilterData" localSheetId="1" hidden="1">case!$A$2:$AD$2</definedName>
   </definedNames>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="Jason Wang - Personal View" guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="2" showComments="commIndAndComment"/>
+    <customWorkbookView name="Cherry (Ying) Xu - Personal View" guid="{7D13FC9B-B344-4E74-B7B7-44B6EA59DFDB}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
+    <customWorkbookView name="Cherry Xu - Personal View" guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="835" activeSheetId="2"/>
     <customWorkbookView name="Xueying Li - Personal View" guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" mergeInterval="0" personalView="1" yWindow="337" windowWidth="1878" windowHeight="703" activeSheetId="1"/>
-    <customWorkbookView name="Cherry Xu - Personal View" guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="835" activeSheetId="2"/>
-    <customWorkbookView name="Cherry (Ying) Xu - Personal View" guid="{7D13FC9B-B344-4E74-B7B7-44B6EA59DFDB}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
-    <customWorkbookView name="Jason Wang - Personal View" guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
   </customWorkbookViews>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="281">
   <si>
     <t>[suite_info]</t>
   </si>
@@ -873,9 +887,6 @@
     <t>cmd = python DEV/tools/runSquish/run_radiant.py</t>
   </si>
   <si>
-    <t>radiant=ng2_3;squish=6.1.0</t>
-  </si>
-  <si>
     <t>gui_flow</t>
   </si>
   <si>
@@ -900,16 +911,25 @@
     <t>tst_toolbar_tool</t>
   </si>
   <si>
-    <t>tst_toolbar_view</t>
-  </si>
-  <si>
-    <t>pn_20_project_navigator_v2.00</t>
+    <t>pn_20_project_navigator_v2.01</t>
+  </si>
+  <si>
+    <t>radiant=ng2_3;squish=6.6.2</t>
+  </si>
+  <si>
+    <t>tst_example_8bit</t>
+  </si>
+  <si>
+    <t>tst_example_16bit</t>
+  </si>
+  <si>
+    <t>8</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.00_ "/>
     <numFmt numFmtId="165" formatCode="0.00_);[Red]\(0.00\)"/>
@@ -1994,7 +2014,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="108">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="12" fillId="7" borderId="7" xfId="13" applyNumberFormat="1" applyProtection="1">
       <alignment vertical="center"/>
@@ -2002,13 +2022,13 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="7" borderId="7" xfId="13" applyNumberFormat="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="47">
@@ -2068,7 +2088,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="16" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="17" xfId="47" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="17" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="18" xfId="47" applyBorder="1" applyAlignment="1">
@@ -2104,22 +2124,13 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="47" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="35" xfId="47" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="35" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="36" xfId="47" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="20" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="24" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="41" xfId="47" applyBorder="1" applyAlignment="1">
@@ -2149,22 +2160,16 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="49" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="47" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="47" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="47" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="47" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="21" fillId="0" borderId="15" xfId="47" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="21" fillId="0" borderId="16" xfId="47" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="17" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="21" fillId="0" borderId="18" xfId="47" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -2179,13 +2184,13 @@
     <xf numFmtId="165" fontId="21" fillId="0" borderId="24" xfId="47" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="42" xfId="47" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="42" xfId="47" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="43" xfId="47" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="43" xfId="47" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="44" xfId="47" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="44" xfId="47" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="21" fillId="0" borderId="21" xfId="47" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -2206,64 +2211,31 @@
     <xf numFmtId="49" fontId="12" fillId="7" borderId="7" xfId="13" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="37" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="18" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="21" xfId="47" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="33" xfId="47" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="37" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="25" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2275,7 +2247,13 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="24" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="35" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="18" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="24" xfId="47" applyBorder="1" applyAlignment="1">
@@ -2295,17 +2273,44 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="37" xfId="48" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="48" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="48" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="47" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" xfId="47" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="21" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="33" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="37" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="37" xfId="47" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="47" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="47" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="47" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="47" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="50">
@@ -2342,19 +2347,19 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Hyperlink 2" xfId="49"/>
+    <cellStyle name="Hyperlink 2" xfId="49" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="41"/>
-    <cellStyle name="Normal 2 2" xfId="47"/>
-    <cellStyle name="Normal 3" xfId="44"/>
-    <cellStyle name="Normal 4" xfId="45"/>
-    <cellStyle name="Normal 5" xfId="46"/>
-    <cellStyle name="Normal 6" xfId="43"/>
-    <cellStyle name="Normal 6 2" xfId="48"/>
-    <cellStyle name="Note 2" xfId="42"/>
+    <cellStyle name="Normal 2" xfId="41" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
+    <cellStyle name="Normal 2 2" xfId="47" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
+    <cellStyle name="Normal 3" xfId="44" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
+    <cellStyle name="Normal 4" xfId="45" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
+    <cellStyle name="Normal 5" xfId="46" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
+    <cellStyle name="Normal 6" xfId="43" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
+    <cellStyle name="Normal 6 2" xfId="48" xr:uid="{00000000-0005-0000-0000-00002C000000}"/>
+    <cellStyle name="Note 2" xfId="42" xr:uid="{00000000-0005-0000-0000-00002D000000}"/>
     <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="16" builtinId="25" customBuiltin="1"/>
@@ -2390,7 +2395,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -4506,7 +4517,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -4561,7 +4578,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3" descr="Add Test Case - TestRail - Mozilla Firefox"/>
+        <xdr:cNvPr id="4" name="Picture 3" descr="Add Test Case - TestRail - Mozilla Firefox">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -4606,7 +4629,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="TextBox 4"/>
+        <xdr:cNvPr id="5" name="TextBox 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -4725,7 +4754,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="6" name="Straight Arrow Connector 5"/>
+        <xdr:cNvPr id="6" name="Straight Arrow Connector 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -4772,7 +4807,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="7" name="Straight Arrow Connector 6"/>
+        <xdr:cNvPr id="7" name="Straight Arrow Connector 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -4808,7 +4849,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{1C0FBCAC-EFCC-4BED-9EF5-4040BE2C87D6}" diskRevisions="1" revisionId="818" version="12">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{9A211320-B0A2-4A74-AB1D-0AB01D61C1CA}" diskRevisions="1" revisionId="827" version="14">
   <header guid="{EF406D44-8062-40DE-A000-69E56EC874B5}" dateTime="2020-10-15T13:42:26" maxSheetId="5" userName="Jason Wang" r:id="rId1">
     <sheetIdMap count="4">
       <sheetId val="1"/>
@@ -4905,6 +4946,22 @@
       <sheetId val="4"/>
     </sheetIdMap>
   </header>
+  <header guid="{B30807FC-B7FE-44F0-94DA-C12FF8777C87}" dateTime="2022-12-14T14:15:40" maxSheetId="5" userName="Jason Wang" r:id="rId13" minRId="819" maxRId="820">
+    <sheetIdMap count="4">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{9A211320-B0A2-4A74-AB1D-0AB01D61C1CA}" dateTime="2022-12-14T14:17:29" maxSheetId="5" userName="Jason Wang" r:id="rId14" minRId="821" maxRId="826">
+    <sheetIdMap count="4">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
@@ -6151,6 +6208,91 @@
       </is>
     </nc>
   </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog13.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="819" sId="1">
+    <oc r="B3" t="inlineStr">
+      <is>
+        <t>pn_20_project_navigator_v2.00</t>
+      </is>
+    </oc>
+    <nc r="B3" t="inlineStr">
+      <is>
+        <t>pn_20_project_navigator_v2.01</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="820" sId="1">
+    <oc r="B8" t="inlineStr">
+      <is>
+        <t>radiant=ng2_3;squish=6.1.0</t>
+      </is>
+    </oc>
+    <nc r="B8" t="inlineStr">
+      <is>
+        <t>radiant=ng2_3;squish=6.6.2</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog14.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="821" sId="2">
+    <oc r="E9" t="inlineStr">
+      <is>
+        <t>tst_toolbar_view</t>
+      </is>
+    </oc>
+    <nc r="E9" t="inlineStr">
+      <is>
+        <t>tst_example_8bit</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="822" sId="2">
+    <nc r="E10" t="inlineStr">
+      <is>
+        <t>tst_example_16bit</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="823" sId="2">
+    <nc r="A10" t="inlineStr">
+      <is>
+        <t>8</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="824" sId="2">
+    <nc r="D10" t="inlineStr">
+      <is>
+        <t>gui_flow</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="825" sId="2" numFmtId="30">
+    <nc r="F10">
+      <v>1</v>
+    </nc>
+  </rcc>
+  <rcc rId="826" sId="2">
+    <nc r="G10" t="inlineStr">
+      <is>
+        <t>GUI test</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" action="delete"/>
+  <rdn rId="0" localSheetId="2" customView="1" name="Z_E811CF45_D5B3_4449_84AE_1514F9E9258F_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>case!$A$2:$AD$2</formula>
+    <oldFormula>case!$A$2:$AD$2</oldFormula>
+  </rdn>
+  <rcv guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" action="add"/>
 </revisions>
 </file>
 
@@ -15975,6 +16117,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -16010,6 +16169,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -16185,11 +16361,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -16220,7 +16396,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -16254,7 +16430,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>268</v>
+        <v>277</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -16275,23 +16451,23 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="BrxOpSv5Qn+u2wRjM+utC6UYLrvUI+Gay+w6zPQp8zz+/5I1udizjqbZ6brqgp9h1Ud3zJVEOn/q/bgrm9i81A==" saltValue="wt9VphKaQ5GnARCLMZGRjA==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <customSheetViews>
-    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
-      <selection activeCell="B4" sqref="B4"/>
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
+      <selection activeCell="B11" sqref="B11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+    </customSheetView>
+    <customSheetView guid="{7D13FC9B-B344-4E74-B7B7-44B6EA59DFDB}">
+      <selection activeCell="C23" sqref="C23"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
     <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}">
       <selection activeCell="B35" sqref="B35"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
-    </customSheetView>
-    <customSheetView guid="{7D13FC9B-B344-4E74-B7B7-44B6EA59DFDB}">
-      <selection activeCell="C23" sqref="C23"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
-      <selection activeCell="B23" sqref="B23"/>
+    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
+      <selection activeCell="B4" sqref="B4"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
     </customSheetView>
@@ -16303,15 +16479,15 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:AD10"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
       <selection pane="topRight" activeCell="A2" sqref="A2"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C14" sqref="C14"/>
+      <selection pane="bottomRight" activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -16344,40 +16520,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" s="3" customFormat="1" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A1" s="67" t="s">
+      <c r="A1" s="62" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="68"/>
-      <c r="K1" s="68"/>
-      <c r="L1" s="68"/>
-      <c r="M1" s="68"/>
-      <c r="N1" s="68"/>
-      <c r="O1" s="68"/>
-      <c r="P1" s="68"/>
-      <c r="Q1" s="68"/>
-      <c r="R1" s="68"/>
-      <c r="S1" s="68"/>
-      <c r="T1" s="68"/>
-      <c r="U1" s="68"/>
-      <c r="V1" s="69"/>
-      <c r="W1" s="70" t="s">
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
+      <c r="I1" s="63"/>
+      <c r="J1" s="63"/>
+      <c r="K1" s="63"/>
+      <c r="L1" s="63"/>
+      <c r="M1" s="63"/>
+      <c r="N1" s="63"/>
+      <c r="O1" s="63"/>
+      <c r="P1" s="63"/>
+      <c r="Q1" s="63"/>
+      <c r="R1" s="63"/>
+      <c r="S1" s="63"/>
+      <c r="T1" s="63"/>
+      <c r="U1" s="63"/>
+      <c r="V1" s="64"/>
+      <c r="W1" s="65" t="s">
         <v>16</v>
       </c>
-      <c r="X1" s="70"/>
-      <c r="Y1" s="70"/>
-      <c r="Z1" s="70"/>
-      <c r="AA1" s="70"/>
-      <c r="AB1" s="70"/>
-      <c r="AC1" s="70"/>
-      <c r="AD1" s="70"/>
+      <c r="X1" s="65"/>
+      <c r="Y1" s="65"/>
+      <c r="Z1" s="65"/>
+      <c r="AA1" s="65"/>
+      <c r="AB1" s="65"/>
+      <c r="AC1" s="65"/>
+      <c r="AD1" s="65"/>
     </row>
     <row r="2" spans="1:30" s="3" customFormat="1" ht="16.5" thickTop="1" thickBot="1">
       <c r="A2" s="1" t="s">
@@ -16476,16 +16652,16 @@
         <v>1</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>269</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>270</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>40</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="4" spans="1:30">
@@ -16493,16 +16669,16 @@
         <v>76</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>40</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="5" spans="1:30">
@@ -16510,16 +16686,16 @@
         <v>75</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>40</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="6" spans="1:30">
@@ -16527,16 +16703,16 @@
         <v>77</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>40</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="7" spans="1:30">
@@ -16544,16 +16720,16 @@
         <v>78</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>40</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="8" spans="1:30">
@@ -16561,16 +16737,16 @@
         <v>79</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>40</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="9" spans="1:30">
@@ -16578,49 +16754,66 @@
         <v>263</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="F9" s="2">
         <v>1</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30">
+      <c r="A10" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="F10" s="2">
+        <v>1</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>270</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="y+CBG6/YKaQ6HsaQYTqaGGAc9K7SdI4KYNN5n42I5k04yiTX0Fn8xQwrYnwNAtl9mwRmr3UcHPCrpySoPgBJNA==" saltValue="2QS/OSgjoJCpqDc5Ec8Idw==" spinCount="100000" sheet="1" objects="1" scenarios="1" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <autoFilter ref="A2:AD2"/>
+  <autoFilter ref="A2:AD2" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <customSheetViews>
-    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" scale="85" showAutoFilter="1">
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" scale="70" showAutoFilter="1">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="H23" sqref="H23"/>
+      <selection pane="bottomRight" activeCell="F12" sqref="F12"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-      <autoFilter ref="A2:Y2"/>
+      <autoFilter ref="A2:AD2" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+    </customSheetView>
+    <customSheetView guid="{7D13FC9B-B344-4E74-B7B7-44B6EA59DFDB}" scale="70" showAutoFilter="1">
+      <pane xSplit="1" ySplit="2" topLeftCell="B57" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="A109" sqref="A109:XFD109"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+      <autoFilter ref="A2:AD2" xr:uid="{DAA659B3-0453-42E2-8680-A77088C89A96}"/>
     </customSheetView>
     <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" scale="85" showAutoFilter="1">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="bottomRight" activeCell="C23" sqref="C23"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
-      <autoFilter ref="A2:Y2"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+      <autoFilter ref="A2:Y2" xr:uid="{CCE242EB-DC18-41B1-AC55-E53E869A4952}"/>
     </customSheetView>
-    <customSheetView guid="{7D13FC9B-B344-4E74-B7B7-44B6EA59DFDB}" scale="70" showAutoFilter="1">
-      <pane xSplit="1" ySplit="2" topLeftCell="B57" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="A109" sqref="A109:XFD109"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
-      <autoFilter ref="A2:AD2"/>
-    </customSheetView>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" scale="70" showAutoFilter="1">
-      <pane xSplit="1" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="AF11" sqref="AF11"/>
+    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" scale="85" showAutoFilter="1">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="H23" sqref="H23"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
-      <autoFilter ref="A2:AD2"/>
+      <autoFilter ref="A2:Y2" xr:uid="{7B13C123-009A-4E78-9B55-D08497079593}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="2">
@@ -16629,7 +16822,7 @@
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AD1 M1:AA1 G1:H1 C1:E1 A1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AD1 M1:AA1 G1:H1 C1:E1 A1" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>
@@ -16638,49 +16831,49 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="8">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000001000000}">
           <x14:formula1>
             <xm:f>description!$F$140:$H$140</xm:f>
           </x14:formula1>
           <xm:sqref>AB1:AB1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000002000000}">
           <x14:formula1>
             <xm:f>description!$F$141:$H$141</xm:f>
           </x14:formula1>
           <xm:sqref>AC1:AC1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000003000000}">
           <x14:formula1>
             <xm:f>description!$F$122:$H$122</xm:f>
           </x14:formula1>
           <xm:sqref>K1:K1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000004000000}">
           <x14:formula1>
             <xm:f>description!$F$121:$K$121</xm:f>
           </x14:formula1>
           <xm:sqref>J1:J1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000005000000}">
           <x14:formula1>
             <xm:f>description!$F$123:$H$123</xm:f>
           </x14:formula1>
           <xm:sqref>L1:L1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000006000000}">
           <x14:formula1>
             <xm:f>description!$E$113:$F$113</xm:f>
           </x14:formula1>
           <xm:sqref>B1:B1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000007000000}">
           <x14:formula1>
             <xm:f>description!$F$117:$H$117</xm:f>
           </x14:formula1>
           <xm:sqref>F1:F1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000008000000}">
           <x14:formula1>
             <xm:f>description!$F$120:$K$120</xm:f>
           </x14:formula1>
@@ -16693,7 +16886,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N241"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
@@ -16758,17 +16951,17 @@
       <c r="E111" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="F111" s="104" t="s">
+      <c r="F111" s="68" t="s">
         <v>87</v>
       </c>
-      <c r="G111" s="105"/>
-      <c r="H111" s="105"/>
-      <c r="I111" s="105"/>
-      <c r="J111" s="105"/>
-      <c r="K111" s="105"/>
-      <c r="L111" s="105"/>
-      <c r="M111" s="105"/>
-      <c r="N111" s="106"/>
+      <c r="G111" s="69"/>
+      <c r="H111" s="69"/>
+      <c r="I111" s="69"/>
+      <c r="J111" s="69"/>
+      <c r="K111" s="69"/>
+      <c r="L111" s="69"/>
+      <c r="M111" s="69"/>
+      <c r="N111" s="70"/>
     </row>
     <row r="112" spans="1:14">
       <c r="A112" s="11" t="s">
@@ -17632,7 +17825,7 @@
       <c r="A147" s="26">
         <v>1</v>
       </c>
-      <c r="B147" s="89" t="s">
+      <c r="B147" s="71" t="s">
         <v>3</v>
       </c>
       <c r="C147" s="27" t="s">
@@ -17658,7 +17851,7 @@
       <c r="A148" s="26">
         <v>2</v>
       </c>
-      <c r="B148" s="90"/>
+      <c r="B148" s="72"/>
       <c r="C148" s="28" t="s">
         <v>136</v>
       </c>
@@ -17680,7 +17873,7 @@
       <c r="A149" s="26">
         <v>3</v>
       </c>
-      <c r="B149" s="90"/>
+      <c r="B149" s="72"/>
       <c r="C149" s="28" t="s">
         <v>9</v>
       </c>
@@ -17700,7 +17893,7 @@
       <c r="A150" s="26">
         <v>4</v>
       </c>
-      <c r="B150" s="90"/>
+      <c r="B150" s="72"/>
       <c r="C150" s="28" t="s">
         <v>138</v>
       </c>
@@ -17724,7 +17917,7 @@
       <c r="A151" s="26">
         <v>5</v>
       </c>
-      <c r="B151" s="90"/>
+      <c r="B151" s="72"/>
       <c r="C151" s="27" t="s">
         <v>140</v>
       </c>
@@ -17748,7 +17941,7 @@
       <c r="A152" s="26">
         <v>6</v>
       </c>
-      <c r="B152" s="90"/>
+      <c r="B152" s="72"/>
       <c r="C152" s="27" t="s">
         <v>144</v>
       </c>
@@ -17772,7 +17965,7 @@
       <c r="A153" s="26">
         <v>7</v>
       </c>
-      <c r="B153" s="90"/>
+      <c r="B153" s="72"/>
       <c r="C153" s="28" t="s">
         <v>147</v>
       </c>
@@ -17794,7 +17987,7 @@
       <c r="A154" s="26">
         <v>8</v>
       </c>
-      <c r="B154" s="90"/>
+      <c r="B154" s="72"/>
       <c r="C154" s="27" t="s">
         <v>148</v>
       </c>
@@ -17818,7 +18011,7 @@
       <c r="A155" s="26">
         <v>9</v>
       </c>
-      <c r="B155" s="90"/>
+      <c r="B155" s="72"/>
       <c r="C155" s="27" t="s">
         <v>149</v>
       </c>
@@ -17842,7 +18035,7 @@
       <c r="A156" s="26">
         <v>10</v>
       </c>
-      <c r="B156" s="90"/>
+      <c r="B156" s="72"/>
       <c r="C156" s="28" t="s">
         <v>150</v>
       </c>
@@ -17866,7 +18059,7 @@
       <c r="A157" s="26">
         <v>11</v>
       </c>
-      <c r="B157" s="90"/>
+      <c r="B157" s="72"/>
       <c r="C157" s="28" t="s">
         <v>151</v>
       </c>
@@ -17890,7 +18083,7 @@
       <c r="A158" s="26">
         <v>12</v>
       </c>
-      <c r="B158" s="90"/>
+      <c r="B158" s="72"/>
       <c r="C158" s="28" t="s">
         <v>153</v>
       </c>
@@ -17912,7 +18105,7 @@
       <c r="A159" s="26">
         <v>13</v>
       </c>
-      <c r="B159" s="84"/>
+      <c r="B159" s="73"/>
       <c r="C159" s="28" t="s">
         <v>56</v>
       </c>
@@ -17936,7 +18129,7 @@
       <c r="A160" s="26">
         <v>14</v>
       </c>
-      <c r="B160" s="80" t="s">
+      <c r="B160" s="66" t="s">
         <v>4</v>
       </c>
       <c r="C160" s="28" t="s">
@@ -17962,7 +18155,7 @@
       <c r="A161" s="26">
         <v>15</v>
       </c>
-      <c r="B161" s="79"/>
+      <c r="B161" s="67"/>
       <c r="C161" s="28" t="s">
         <v>161</v>
       </c>
@@ -17986,7 +18179,7 @@
       <c r="A162" s="26">
         <v>16</v>
       </c>
-      <c r="B162" s="89" t="s">
+      <c r="B162" s="71" t="s">
         <v>5</v>
       </c>
       <c r="C162" s="28" t="s">
@@ -18010,7 +18203,7 @@
       <c r="A163" s="26">
         <v>17</v>
       </c>
-      <c r="B163" s="107"/>
+      <c r="B163" s="74"/>
       <c r="C163" s="27" t="s">
         <v>165</v>
       </c>
@@ -18032,7 +18225,7 @@
       <c r="A164" s="26">
         <v>18</v>
       </c>
-      <c r="B164" s="84"/>
+      <c r="B164" s="73"/>
       <c r="C164" s="27" t="s">
         <v>167</v>
       </c>
@@ -18052,7 +18245,7 @@
       <c r="A165" s="26">
         <v>19</v>
       </c>
-      <c r="B165" s="80" t="s">
+      <c r="B165" s="66" t="s">
         <v>6</v>
       </c>
       <c r="C165" s="28" t="s">
@@ -18076,7 +18269,7 @@
       <c r="A166" s="26">
         <v>20</v>
       </c>
-      <c r="B166" s="79"/>
+      <c r="B166" s="67"/>
       <c r="C166" s="28" t="s">
         <v>172</v>
       </c>
@@ -18096,7 +18289,7 @@
       <c r="A167" s="26">
         <v>21</v>
       </c>
-      <c r="B167" s="79"/>
+      <c r="B167" s="67"/>
       <c r="C167" s="28" t="s">
         <v>173</v>
       </c>
@@ -18116,7 +18309,7 @@
       <c r="A168" s="26">
         <v>22</v>
       </c>
-      <c r="B168" s="79"/>
+      <c r="B168" s="67"/>
       <c r="C168" s="28" t="s">
         <v>174</v>
       </c>
@@ -18136,7 +18329,7 @@
       <c r="A169" s="26">
         <v>23</v>
       </c>
-      <c r="B169" s="79"/>
+      <c r="B169" s="67"/>
       <c r="C169" s="28" t="s">
         <v>175</v>
       </c>
@@ -18156,7 +18349,7 @@
       <c r="A170" s="26">
         <v>24</v>
       </c>
-      <c r="B170" s="79"/>
+      <c r="B170" s="67"/>
       <c r="C170" s="28" t="s">
         <v>176</v>
       </c>
@@ -18176,7 +18369,7 @@
       <c r="A171" s="26">
         <v>25</v>
       </c>
-      <c r="B171" s="79"/>
+      <c r="B171" s="67"/>
       <c r="C171" s="28" t="s">
         <v>177</v>
       </c>
@@ -18196,7 +18389,7 @@
       <c r="A172" s="26">
         <v>26</v>
       </c>
-      <c r="B172" s="79"/>
+      <c r="B172" s="67"/>
       <c r="C172" s="28" t="s">
         <v>41</v>
       </c>
@@ -18216,7 +18409,7 @@
       <c r="A173" s="26">
         <v>27</v>
       </c>
-      <c r="B173" s="80" t="s">
+      <c r="B173" s="66" t="s">
         <v>7</v>
       </c>
       <c r="C173" s="28" t="s">
@@ -18240,7 +18433,7 @@
       <c r="A174" s="26">
         <v>28</v>
       </c>
-      <c r="B174" s="79"/>
+      <c r="B174" s="67"/>
       <c r="C174" s="27" t="s">
         <v>181</v>
       </c>
@@ -18262,7 +18455,7 @@
       <c r="A175" s="26">
         <v>29</v>
       </c>
-      <c r="B175" s="79"/>
+      <c r="B175" s="67"/>
       <c r="C175" s="28" t="s">
         <v>184</v>
       </c>
@@ -18284,7 +18477,7 @@
       <c r="A176" s="26">
         <v>30</v>
       </c>
-      <c r="B176" s="89" t="s">
+      <c r="B176" s="71" t="s">
         <v>8</v>
       </c>
       <c r="C176" s="28" t="s">
@@ -18310,7 +18503,7 @@
       <c r="A177" s="31">
         <v>31</v>
       </c>
-      <c r="B177" s="90"/>
+      <c r="B177" s="72"/>
       <c r="C177" s="32" t="s">
         <v>189</v>
       </c>
@@ -18334,7 +18527,7 @@
       <c r="A178" s="23">
         <v>32</v>
       </c>
-      <c r="B178" s="91" t="s">
+      <c r="B178" s="75" t="s">
         <v>191</v>
       </c>
       <c r="C178" s="33" t="s">
@@ -18358,7 +18551,7 @@
       <c r="A179" s="26">
         <v>33</v>
       </c>
-      <c r="B179" s="92"/>
+      <c r="B179" s="76"/>
       <c r="C179" s="27" t="s">
         <v>195</v>
       </c>
@@ -18380,7 +18573,7 @@
       <c r="A180" s="26">
         <v>34</v>
       </c>
-      <c r="B180" s="93"/>
+      <c r="B180" s="77"/>
       <c r="C180" s="34" t="s">
         <v>198</v>
       </c>
@@ -18402,7 +18595,7 @@
       <c r="A181" s="31">
         <v>35</v>
       </c>
-      <c r="B181" s="93"/>
+      <c r="B181" s="77"/>
       <c r="C181" s="34" t="s">
         <v>199</v>
       </c>
@@ -18424,17 +18617,17 @@
       <c r="A182" s="31">
         <v>36</v>
       </c>
-      <c r="B182" s="93"/>
+      <c r="B182" s="77"/>
       <c r="C182" s="34" t="s">
         <v>202</v>
       </c>
-      <c r="D182" s="42" t="s">
+      <c r="D182" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="E182" s="42" t="s">
+      <c r="E182" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="F182" s="42"/>
+      <c r="F182" s="32"/>
       <c r="G182" s="34" t="s">
         <v>260</v>
       </c>
@@ -18444,15 +18637,15 @@
       <c r="A183" s="31">
         <v>37</v>
       </c>
-      <c r="B183" s="93"/>
+      <c r="B183" s="77"/>
       <c r="C183" s="34" t="s">
         <v>254</v>
       </c>
-      <c r="D183" s="42" t="s">
+      <c r="D183" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="E183" s="42"/>
-      <c r="F183" s="42" t="s">
+      <c r="E183" s="32"/>
+      <c r="F183" s="32" t="s">
         <v>255</v>
       </c>
       <c r="G183" s="34" t="s">
@@ -18466,7 +18659,7 @@
       <c r="A184" s="35">
         <v>38</v>
       </c>
-      <c r="B184" s="88"/>
+      <c r="B184" s="78"/>
       <c r="C184" s="36" t="s">
         <v>258</v>
       </c>
@@ -18493,7 +18686,7 @@
       </c>
     </row>
     <row r="186" spans="1:8">
-      <c r="B186" s="37" t="s">
+      <c r="B186" s="6" t="s">
         <v>205</v>
       </c>
     </row>
@@ -18514,280 +18707,280 @@
       <c r="A198" s="9" t="s">
         <v>209</v>
       </c>
-      <c r="B198" s="38" t="s">
+      <c r="B198" s="37" t="s">
         <v>210</v>
       </c>
-      <c r="C198" s="94" t="s">
+      <c r="C198" s="79" t="s">
         <v>44</v>
       </c>
-      <c r="D198" s="94"/>
-      <c r="E198" s="94"/>
-      <c r="F198" s="39" t="s">
+      <c r="D198" s="79"/>
+      <c r="E198" s="79"/>
+      <c r="F198" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="G198" s="40" t="s">
+      <c r="G198" s="38" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="199" spans="1:7">
-      <c r="A199" s="77" t="s">
+      <c r="A199" s="80" t="s">
         <v>212</v>
       </c>
-      <c r="B199" s="79" t="s">
+      <c r="B199" s="67" t="s">
         <v>213</v>
       </c>
-      <c r="C199" s="96" t="s">
+      <c r="C199" s="82" t="s">
         <v>57</v>
       </c>
-      <c r="D199" s="97"/>
-      <c r="E199" s="97"/>
+      <c r="D199" s="83"/>
+      <c r="E199" s="83"/>
       <c r="F199" s="28" t="s">
         <v>214</v>
       </c>
-      <c r="G199" s="41" t="s">
+      <c r="G199" s="39" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="200" spans="1:7">
-      <c r="A200" s="77"/>
-      <c r="B200" s="95"/>
-      <c r="C200" s="98" t="s">
+      <c r="A200" s="80"/>
+      <c r="B200" s="81"/>
+      <c r="C200" s="84" t="s">
         <v>57</v>
       </c>
-      <c r="D200" s="99"/>
-      <c r="E200" s="99"/>
+      <c r="D200" s="85"/>
+      <c r="E200" s="85"/>
       <c r="F200" s="32" t="s">
         <v>215</v>
       </c>
-      <c r="G200" s="43" t="s">
+      <c r="G200" s="40" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="201" spans="1:7">
-      <c r="A201" s="77"/>
-      <c r="B201" s="79" t="s">
+      <c r="A201" s="80"/>
+      <c r="B201" s="67" t="s">
         <v>216</v>
       </c>
-      <c r="C201" s="100" t="s">
+      <c r="C201" s="86" t="s">
         <v>217</v>
       </c>
-      <c r="D201" s="100"/>
-      <c r="E201" s="100"/>
+      <c r="D201" s="86"/>
+      <c r="E201" s="86"/>
       <c r="F201" s="28" t="s">
         <v>214</v>
       </c>
-      <c r="G201" s="41" t="s">
+      <c r="G201" s="39" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="202" spans="1:7">
-      <c r="A202" s="77"/>
-      <c r="B202" s="79"/>
-      <c r="C202" s="98" t="s">
+      <c r="A202" s="80"/>
+      <c r="B202" s="67"/>
+      <c r="C202" s="84" t="s">
         <v>217</v>
       </c>
-      <c r="D202" s="98"/>
-      <c r="E202" s="98"/>
+      <c r="D202" s="84"/>
+      <c r="E202" s="84"/>
       <c r="F202" s="28" t="s">
         <v>215</v>
       </c>
-      <c r="G202" s="41" t="s">
+      <c r="G202" s="39" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="203" spans="1:7">
-      <c r="A203" s="77"/>
-      <c r="B203" s="95" t="s">
+      <c r="A203" s="80"/>
+      <c r="B203" s="81" t="s">
         <v>218</v>
       </c>
-      <c r="C203" s="101" t="s">
+      <c r="C203" s="87" t="s">
         <v>57</v>
       </c>
-      <c r="D203" s="102"/>
-      <c r="E203" s="103"/>
+      <c r="D203" s="88"/>
+      <c r="E203" s="89"/>
       <c r="F203" s="28" t="s">
         <v>214</v>
       </c>
-      <c r="G203" s="41" t="s">
+      <c r="G203" s="39" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="204" spans="1:7">
-      <c r="A204" s="77"/>
-      <c r="B204" s="84"/>
-      <c r="C204" s="101" t="s">
+      <c r="A204" s="80"/>
+      <c r="B204" s="73"/>
+      <c r="C204" s="87" t="s">
         <v>57</v>
       </c>
-      <c r="D204" s="102"/>
-      <c r="E204" s="103"/>
+      <c r="D204" s="88"/>
+      <c r="E204" s="89"/>
       <c r="F204" s="28" t="s">
         <v>215</v>
       </c>
-      <c r="G204" s="41" t="s">
+      <c r="G204" s="39" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="205" spans="1:7">
-      <c r="A205" s="77"/>
-      <c r="B205" s="79" t="s">
+      <c r="A205" s="80"/>
+      <c r="B205" s="67" t="s">
         <v>219</v>
       </c>
-      <c r="C205" s="100" t="s">
+      <c r="C205" s="86" t="s">
         <v>220</v>
       </c>
-      <c r="D205" s="100"/>
-      <c r="E205" s="100"/>
+      <c r="D205" s="86"/>
+      <c r="E205" s="86"/>
       <c r="F205" s="28" t="s">
         <v>214</v>
       </c>
-      <c r="G205" s="41" t="s">
+      <c r="G205" s="39" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="206" spans="1:7">
-      <c r="A206" s="77"/>
-      <c r="B206" s="79"/>
-      <c r="C206" s="100" t="s">
+      <c r="A206" s="80"/>
+      <c r="B206" s="67"/>
+      <c r="C206" s="86" t="s">
         <v>220</v>
       </c>
-      <c r="D206" s="100"/>
-      <c r="E206" s="100"/>
+      <c r="D206" s="86"/>
+      <c r="E206" s="86"/>
       <c r="F206" s="28" t="s">
         <v>215</v>
       </c>
-      <c r="G206" s="41" t="s">
+      <c r="G206" s="39" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="207" spans="1:7">
-      <c r="A207" s="77" t="s">
+      <c r="A207" s="80" t="s">
         <v>221</v>
       </c>
-      <c r="B207" s="79" t="s">
+      <c r="B207" s="67" t="s">
         <v>222</v>
       </c>
-      <c r="C207" s="80" t="s">
+      <c r="C207" s="66" t="s">
         <v>45</v>
       </c>
-      <c r="D207" s="79"/>
-      <c r="E207" s="79"/>
+      <c r="D207" s="67"/>
+      <c r="E207" s="67"/>
       <c r="F207" s="28" t="s">
         <v>214</v>
       </c>
-      <c r="G207" s="41" t="s">
+      <c r="G207" s="39" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="208" spans="1:7">
-      <c r="A208" s="77"/>
-      <c r="B208" s="79"/>
-      <c r="C208" s="79" t="s">
+      <c r="A208" s="80"/>
+      <c r="B208" s="67"/>
+      <c r="C208" s="67" t="s">
         <v>46</v>
       </c>
-      <c r="D208" s="79"/>
-      <c r="E208" s="79"/>
+      <c r="D208" s="67"/>
+      <c r="E208" s="67"/>
       <c r="F208" s="28" t="s">
         <v>215</v>
       </c>
-      <c r="G208" s="41" t="s">
+      <c r="G208" s="39" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="209" spans="1:7">
-      <c r="A209" s="77"/>
-      <c r="B209" s="79" t="s">
+      <c r="A209" s="80"/>
+      <c r="B209" s="67" t="s">
         <v>224</v>
       </c>
-      <c r="C209" s="79" t="s">
+      <c r="C209" s="67" t="s">
         <v>47</v>
       </c>
-      <c r="D209" s="79"/>
-      <c r="E209" s="79"/>
+      <c r="D209" s="67"/>
+      <c r="E209" s="67"/>
       <c r="F209" s="28" t="s">
         <v>214</v>
       </c>
-      <c r="G209" s="41" t="s">
+      <c r="G209" s="39" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="210" spans="1:7">
-      <c r="A210" s="77"/>
-      <c r="B210" s="79"/>
-      <c r="C210" s="79" t="s">
+      <c r="A210" s="80"/>
+      <c r="B210" s="67"/>
+      <c r="C210" s="67" t="s">
         <v>48</v>
       </c>
-      <c r="D210" s="79"/>
-      <c r="E210" s="79"/>
+      <c r="D210" s="67"/>
+      <c r="E210" s="67"/>
       <c r="F210" s="28" t="s">
         <v>215</v>
       </c>
-      <c r="G210" s="41" t="s">
+      <c r="G210" s="39" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="211" spans="1:7">
-      <c r="A211" s="77" t="s">
+      <c r="A211" s="80" t="s">
         <v>225</v>
       </c>
-      <c r="B211" s="79" t="s">
+      <c r="B211" s="67" t="s">
         <v>226</v>
       </c>
-      <c r="C211" s="80" t="s">
+      <c r="C211" s="66" t="s">
         <v>49</v>
       </c>
-      <c r="D211" s="79"/>
-      <c r="E211" s="79"/>
+      <c r="D211" s="67"/>
+      <c r="E211" s="67"/>
       <c r="F211" s="28" t="s">
         <v>214</v>
       </c>
-      <c r="G211" s="41" t="s">
+      <c r="G211" s="39" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="212" spans="1:7">
-      <c r="A212" s="77"/>
-      <c r="B212" s="79"/>
-      <c r="C212" s="79" t="s">
+      <c r="A212" s="80"/>
+      <c r="B212" s="67"/>
+      <c r="C212" s="67" t="s">
         <v>50</v>
       </c>
-      <c r="D212" s="79"/>
-      <c r="E212" s="79"/>
+      <c r="D212" s="67"/>
+      <c r="E212" s="67"/>
       <c r="F212" s="28" t="s">
         <v>215</v>
       </c>
-      <c r="G212" s="41" t="s">
+      <c r="G212" s="39" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="213" spans="1:7">
-      <c r="A213" s="77"/>
-      <c r="B213" s="79" t="s">
+      <c r="A213" s="80"/>
+      <c r="B213" s="67" t="s">
         <v>227</v>
       </c>
-      <c r="C213" s="80" t="s">
+      <c r="C213" s="66" t="s">
         <v>228</v>
       </c>
-      <c r="D213" s="79"/>
-      <c r="E213" s="79"/>
+      <c r="D213" s="67"/>
+      <c r="E213" s="67"/>
       <c r="F213" s="28" t="s">
         <v>214</v>
       </c>
-      <c r="G213" s="41" t="s">
+      <c r="G213" s="39" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="214" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A214" s="78"/>
-      <c r="B214" s="81"/>
-      <c r="C214" s="81" t="s">
+      <c r="A214" s="91"/>
+      <c r="B214" s="92"/>
+      <c r="C214" s="92" t="s">
         <v>229</v>
       </c>
-      <c r="D214" s="81"/>
-      <c r="E214" s="81"/>
+      <c r="D214" s="92"/>
+      <c r="E214" s="92"/>
       <c r="F214" s="36" t="s">
         <v>215</v>
       </c>
-      <c r="G214" s="44" t="s">
+      <c r="G214" s="41" t="s">
         <v>63</v>
       </c>
     </row>
@@ -18795,60 +18988,43 @@
       <c r="A215" s="6" t="s">
         <v>230</v>
       </c>
-      <c r="C215" s="37"/>
-      <c r="D215" s="37"/>
-      <c r="E215" s="37"/>
-      <c r="F215" s="37"/>
-    </row>
-    <row r="216" spans="1:7">
-      <c r="C216" s="37"/>
-      <c r="D216" s="37"/>
-      <c r="E216" s="37"/>
-    </row>
-    <row r="217" spans="1:7">
-      <c r="C217" s="37"/>
-      <c r="D217" s="37"/>
-      <c r="E217" s="37"/>
     </row>
     <row r="218" spans="1:7" ht="15.75" thickBot="1">
       <c r="A218" s="6" t="s">
         <v>231</v>
       </c>
-      <c r="C218" s="37"/>
-      <c r="D218" s="37"/>
-      <c r="E218" s="37"/>
     </row>
     <row r="219" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A219" s="45" t="s">
+      <c r="A219" s="42" t="s">
         <v>232</v>
       </c>
-      <c r="B219" s="82" t="s">
+      <c r="B219" s="93" t="s">
         <v>52</v>
       </c>
-      <c r="C219" s="82"/>
-      <c r="D219" s="82"/>
-      <c r="E219" s="82"/>
-      <c r="F219" s="46" t="s">
+      <c r="C219" s="93"/>
+      <c r="D219" s="93"/>
+      <c r="E219" s="93"/>
+      <c r="F219" s="43" t="s">
         <v>233</v>
       </c>
-      <c r="G219" s="47" t="s">
+      <c r="G219" s="44" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="220" spans="1:7" ht="93" customHeight="1">
-      <c r="A220" s="48" t="s">
+      <c r="A220" s="45" t="s">
         <v>235</v>
       </c>
-      <c r="B220" s="83" t="s">
+      <c r="B220" s="94" t="s">
         <v>236</v>
       </c>
-      <c r="C220" s="84"/>
-      <c r="D220" s="84"/>
-      <c r="E220" s="84"/>
-      <c r="F220" s="49" t="s">
+      <c r="C220" s="73"/>
+      <c r="D220" s="73"/>
+      <c r="E220" s="73"/>
+      <c r="F220" s="46" t="s">
         <v>111</v>
       </c>
-      <c r="G220" s="50" t="s">
+      <c r="G220" s="47" t="s">
         <v>63</v>
       </c>
     </row>
@@ -18856,12 +19032,12 @@
       <c r="A221" s="14" t="s">
         <v>237</v>
       </c>
-      <c r="B221" s="85" t="s">
+      <c r="B221" s="95" t="s">
         <v>238</v>
       </c>
-      <c r="C221" s="86"/>
-      <c r="D221" s="86"/>
-      <c r="E221" s="87"/>
+      <c r="C221" s="96"/>
+      <c r="D221" s="96"/>
+      <c r="E221" s="97"/>
       <c r="F221" s="15" t="s">
         <v>63</v>
       </c>
@@ -18873,12 +19049,12 @@
       <c r="A222" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="B222" s="85" t="s">
+      <c r="B222" s="95" t="s">
         <v>239</v>
       </c>
-      <c r="C222" s="86"/>
-      <c r="D222" s="86"/>
-      <c r="E222" s="87"/>
+      <c r="C222" s="96"/>
+      <c r="D222" s="96"/>
+      <c r="E222" s="97"/>
       <c r="F222" s="18" t="s">
         <v>63</v>
       </c>
@@ -18890,12 +19066,12 @@
       <c r="A223" s="20" t="s">
         <v>240</v>
       </c>
-      <c r="B223" s="88" t="s">
+      <c r="B223" s="78" t="s">
         <v>241</v>
       </c>
-      <c r="C223" s="81"/>
-      <c r="D223" s="81"/>
-      <c r="E223" s="81"/>
+      <c r="C223" s="92"/>
+      <c r="D223" s="92"/>
+      <c r="E223" s="92"/>
       <c r="F223" s="21" t="s">
         <v>63</v>
       </c>
@@ -18904,7 +19080,7 @@
       </c>
     </row>
     <row r="224" spans="1:7">
-      <c r="C224" s="51"/>
+      <c r="C224" s="48"/>
     </row>
     <row r="226" spans="1:7" ht="15.75" thickBot="1">
       <c r="A226" s="6" t="s">
@@ -18915,280 +19091,303 @@
       <c r="A227" s="9" t="s">
         <v>243</v>
       </c>
-      <c r="B227" s="38" t="s">
+      <c r="B227" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="C227" s="52" t="s">
+      <c r="C227" s="49" t="s">
         <v>53</v>
       </c>
-      <c r="D227" s="53" t="s">
+      <c r="D227" s="50" t="s">
         <v>52</v>
       </c>
-      <c r="E227" s="53"/>
-      <c r="F227" s="54"/>
-      <c r="G227" s="40" t="s">
+      <c r="E227" s="50"/>
+      <c r="F227" s="10"/>
+      <c r="G227" s="38" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="228" spans="1:7">
-      <c r="A228" s="55">
+      <c r="A228" s="51">
         <v>42682</v>
       </c>
-      <c r="B228" s="56">
+      <c r="B228" s="52">
         <v>1.04</v>
       </c>
       <c r="C228" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="D228" s="76" t="s">
+      <c r="D228" s="90" t="s">
         <v>54</v>
       </c>
-      <c r="E228" s="76"/>
-      <c r="F228" s="76"/>
-      <c r="G228" s="57"/>
+      <c r="E228" s="90"/>
+      <c r="F228" s="90"/>
+      <c r="G228" s="25"/>
     </row>
     <row r="229" spans="1:7">
-      <c r="A229" s="58">
+      <c r="A229" s="53">
         <v>42692</v>
       </c>
-      <c r="B229" s="59">
+      <c r="B229" s="54">
         <v>1.05</v>
       </c>
       <c r="C229" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="D229" s="75" t="s">
+      <c r="D229" s="102" t="s">
         <v>55</v>
       </c>
-      <c r="E229" s="75"/>
-      <c r="F229" s="75"/>
-      <c r="G229" s="41"/>
+      <c r="E229" s="102"/>
+      <c r="F229" s="102"/>
+      <c r="G229" s="39"/>
     </row>
     <row r="230" spans="1:7">
-      <c r="A230" s="58">
+      <c r="A230" s="53">
         <v>42955</v>
       </c>
-      <c r="B230" s="59">
+      <c r="B230" s="54">
         <v>1.06</v>
       </c>
       <c r="C230" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="D230" s="75" t="s">
+      <c r="D230" s="102" t="s">
         <v>245</v>
       </c>
-      <c r="E230" s="75"/>
-      <c r="F230" s="75"/>
-      <c r="G230" s="41"/>
+      <c r="E230" s="102"/>
+      <c r="F230" s="102"/>
+      <c r="G230" s="39"/>
     </row>
     <row r="231" spans="1:7">
-      <c r="A231" s="58">
+      <c r="A231" s="53">
         <v>42991</v>
       </c>
-      <c r="B231" s="59">
+      <c r="B231" s="54">
         <v>1.07</v>
       </c>
       <c r="C231" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="D231" s="75" t="s">
+      <c r="D231" s="102" t="s">
         <v>246</v>
       </c>
-      <c r="E231" s="75"/>
-      <c r="F231" s="75"/>
-      <c r="G231" s="41"/>
+      <c r="E231" s="102"/>
+      <c r="F231" s="102"/>
+      <c r="G231" s="39"/>
     </row>
     <row r="232" spans="1:7">
-      <c r="A232" s="58">
+      <c r="A232" s="53">
         <v>43026</v>
       </c>
-      <c r="B232" s="59">
+      <c r="B232" s="54">
         <v>1.08</v>
       </c>
       <c r="C232" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="D232" s="75" t="s">
+      <c r="D232" s="102" t="s">
         <v>247</v>
       </c>
-      <c r="E232" s="75"/>
-      <c r="F232" s="75"/>
-      <c r="G232" s="41"/>
+      <c r="E232" s="102"/>
+      <c r="F232" s="102"/>
+      <c r="G232" s="39"/>
     </row>
     <row r="233" spans="1:7">
-      <c r="A233" s="58">
+      <c r="A233" s="53">
         <v>43069</v>
       </c>
-      <c r="B233" s="59">
+      <c r="B233" s="54">
         <v>1.0900000000000001</v>
       </c>
       <c r="C233" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="D233" s="75" t="s">
+      <c r="D233" s="102" t="s">
         <v>248</v>
       </c>
-      <c r="E233" s="75"/>
-      <c r="F233" s="75"/>
-      <c r="G233" s="41"/>
+      <c r="E233" s="102"/>
+      <c r="F233" s="102"/>
+      <c r="G233" s="39"/>
     </row>
     <row r="234" spans="1:7">
-      <c r="A234" s="60">
+      <c r="A234" s="55">
         <v>43248</v>
       </c>
-      <c r="B234" s="61">
+      <c r="B234" s="56">
         <v>1.1000000000000001</v>
       </c>
       <c r="C234" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="D234" s="71" t="s">
+      <c r="D234" s="98" t="s">
         <v>64</v>
       </c>
-      <c r="E234" s="72"/>
-      <c r="F234" s="73"/>
-      <c r="G234" s="43"/>
+      <c r="E234" s="99"/>
+      <c r="F234" s="100"/>
+      <c r="G234" s="40"/>
     </row>
     <row r="235" spans="1:7">
-      <c r="A235" s="60">
+      <c r="A235" s="55">
         <v>43339</v>
       </c>
-      <c r="B235" s="61">
+      <c r="B235" s="56">
         <v>1.1100000000000001</v>
       </c>
       <c r="C235" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="D235" s="71" t="s">
+      <c r="D235" s="98" t="s">
         <v>65</v>
       </c>
-      <c r="E235" s="72"/>
-      <c r="F235" s="73"/>
-      <c r="G235" s="43"/>
+      <c r="E235" s="99"/>
+      <c r="F235" s="100"/>
+      <c r="G235" s="40"/>
     </row>
     <row r="236" spans="1:7">
-      <c r="A236" s="60">
+      <c r="A236" s="55">
         <v>43542</v>
       </c>
-      <c r="B236" s="61">
+      <c r="B236" s="56">
         <v>1.1200000000000001</v>
       </c>
       <c r="C236" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="D236" s="71" t="s">
+      <c r="D236" s="98" t="s">
         <v>69</v>
       </c>
-      <c r="E236" s="72"/>
-      <c r="F236" s="73"/>
-      <c r="G236" s="43"/>
+      <c r="E236" s="99"/>
+      <c r="F236" s="100"/>
+      <c r="G236" s="40"/>
     </row>
     <row r="237" spans="1:7">
-      <c r="A237" s="60">
+      <c r="A237" s="55">
         <v>43599</v>
       </c>
-      <c r="B237" s="61">
+      <c r="B237" s="56">
         <v>1.1299999999999999</v>
       </c>
       <c r="C237" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="D237" s="62" t="s">
+      <c r="D237" s="57" t="s">
         <v>70</v>
       </c>
-      <c r="E237" s="63"/>
-      <c r="F237" s="64"/>
-      <c r="G237" s="43"/>
+      <c r="E237" s="58"/>
+      <c r="F237" s="59"/>
+      <c r="G237" s="40"/>
     </row>
     <row r="238" spans="1:7">
-      <c r="A238" s="60">
+      <c r="A238" s="55">
         <v>43643</v>
       </c>
-      <c r="B238" s="61">
+      <c r="B238" s="56">
         <v>1.1399999999999999</v>
       </c>
       <c r="C238" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="D238" s="62" t="s">
+      <c r="D238" s="57" t="s">
         <v>73</v>
       </c>
-      <c r="E238" s="63"/>
-      <c r="F238" s="64"/>
-      <c r="G238" s="43"/>
+      <c r="E238" s="58"/>
+      <c r="F238" s="59"/>
+      <c r="G238" s="40"/>
     </row>
     <row r="239" spans="1:7">
-      <c r="A239" s="60">
+      <c r="A239" s="55">
         <v>43894</v>
       </c>
-      <c r="B239" s="61">
+      <c r="B239" s="56">
         <v>1.1499999999999999</v>
       </c>
       <c r="C239" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="D239" s="62" t="s">
+      <c r="D239" s="57" t="s">
         <v>74</v>
       </c>
-      <c r="E239" s="63"/>
-      <c r="F239" s="64"/>
-      <c r="G239" s="43"/>
+      <c r="E239" s="58"/>
+      <c r="F239" s="59"/>
+      <c r="G239" s="40"/>
     </row>
     <row r="240" spans="1:7">
-      <c r="A240" s="60">
+      <c r="A240" s="55">
         <v>44017</v>
       </c>
-      <c r="B240" s="61">
+      <c r="B240" s="56">
         <v>1.1599999999999999</v>
       </c>
-      <c r="C240" s="42" t="s">
+      <c r="C240" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="D240" s="62" t="s">
+      <c r="D240" s="57" t="s">
         <v>249</v>
       </c>
-      <c r="E240" s="63"/>
-      <c r="F240" s="64"/>
-      <c r="G240" s="43"/>
+      <c r="E240" s="58"/>
+      <c r="F240" s="59"/>
+      <c r="G240" s="40"/>
     </row>
     <row r="241" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A241" s="65">
+      <c r="A241" s="60">
         <v>44118</v>
       </c>
-      <c r="B241" s="66">
+      <c r="B241" s="61">
         <v>1.17</v>
       </c>
       <c r="C241" s="36" t="s">
         <v>51</v>
       </c>
-      <c r="D241" s="74" t="s">
+      <c r="D241" s="101" t="s">
         <v>261</v>
       </c>
-      <c r="E241" s="74"/>
-      <c r="F241" s="74"/>
-      <c r="G241" s="44"/>
+      <c r="E241" s="101"/>
+      <c r="F241" s="101"/>
+      <c r="G241" s="41"/>
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="ap+vydlQsTivses2kTOZJOfe+E+ofk18ovQVkbwX/cy/2QzQqNYlkd6ZRwhTqYv60tXLJj9O4rjHfeOPlaqbDA==" saltValue="NIz07f4XZ+x9XJy8gC1img==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <customSheetViews>
-    <customSheetView guid="{7D13FC9B-B344-4E74-B7B7-44B6EA59DFDB}" scale="115" topLeftCell="A172">
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" scale="115">
       <selection activeCell="C180" sqref="C180"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
     </customSheetView>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" scale="115">
+    <customSheetView guid="{7D13FC9B-B344-4E74-B7B7-44B6EA59DFDB}" scale="115" topLeftCell="A172">
       <selection activeCell="C180" sqref="C180"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="51">
-    <mergeCell ref="B173:B175"/>
-    <mergeCell ref="F111:N111"/>
-    <mergeCell ref="B147:B159"/>
-    <mergeCell ref="B160:B161"/>
-    <mergeCell ref="B162:B164"/>
-    <mergeCell ref="B165:B172"/>
+    <mergeCell ref="D235:F235"/>
+    <mergeCell ref="D236:F236"/>
+    <mergeCell ref="D241:F241"/>
+    <mergeCell ref="D229:F229"/>
+    <mergeCell ref="D230:F230"/>
+    <mergeCell ref="D231:F231"/>
+    <mergeCell ref="D232:F232"/>
+    <mergeCell ref="D233:F233"/>
+    <mergeCell ref="D234:F234"/>
+    <mergeCell ref="D228:F228"/>
+    <mergeCell ref="A211:A214"/>
+    <mergeCell ref="B211:B212"/>
+    <mergeCell ref="C211:E211"/>
+    <mergeCell ref="C212:E212"/>
+    <mergeCell ref="B213:B214"/>
+    <mergeCell ref="C213:E213"/>
+    <mergeCell ref="C214:E214"/>
+    <mergeCell ref="B219:E219"/>
+    <mergeCell ref="B220:E220"/>
+    <mergeCell ref="B221:E221"/>
+    <mergeCell ref="B222:E222"/>
+    <mergeCell ref="B223:E223"/>
+    <mergeCell ref="A207:A210"/>
+    <mergeCell ref="B207:B208"/>
+    <mergeCell ref="C207:E207"/>
+    <mergeCell ref="C208:E208"/>
+    <mergeCell ref="B209:B210"/>
+    <mergeCell ref="C209:E209"/>
+    <mergeCell ref="C210:E210"/>
     <mergeCell ref="B176:B177"/>
     <mergeCell ref="B178:B184"/>
     <mergeCell ref="C198:E198"/>
@@ -19205,35 +19404,12 @@
     <mergeCell ref="B205:B206"/>
     <mergeCell ref="C205:E205"/>
     <mergeCell ref="C206:E206"/>
-    <mergeCell ref="A207:A210"/>
-    <mergeCell ref="B207:B208"/>
-    <mergeCell ref="C207:E207"/>
-    <mergeCell ref="C208:E208"/>
-    <mergeCell ref="B209:B210"/>
-    <mergeCell ref="C209:E209"/>
-    <mergeCell ref="C210:E210"/>
-    <mergeCell ref="D228:F228"/>
-    <mergeCell ref="A211:A214"/>
-    <mergeCell ref="B211:B212"/>
-    <mergeCell ref="C211:E211"/>
-    <mergeCell ref="C212:E212"/>
-    <mergeCell ref="B213:B214"/>
-    <mergeCell ref="C213:E213"/>
-    <mergeCell ref="C214:E214"/>
-    <mergeCell ref="B219:E219"/>
-    <mergeCell ref="B220:E220"/>
-    <mergeCell ref="B221:E221"/>
-    <mergeCell ref="B222:E222"/>
-    <mergeCell ref="B223:E223"/>
-    <mergeCell ref="D235:F235"/>
-    <mergeCell ref="D236:F236"/>
-    <mergeCell ref="D241:F241"/>
-    <mergeCell ref="D229:F229"/>
-    <mergeCell ref="D230:F230"/>
-    <mergeCell ref="D231:F231"/>
-    <mergeCell ref="D232:F232"/>
-    <mergeCell ref="D233:F233"/>
-    <mergeCell ref="D234:F234"/>
+    <mergeCell ref="B173:B175"/>
+    <mergeCell ref="F111:N111"/>
+    <mergeCell ref="B147:B159"/>
+    <mergeCell ref="B160:B161"/>
+    <mergeCell ref="B162:B164"/>
+    <mergeCell ref="B165:B172"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -19242,7 +19418,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -19256,18 +19432,18 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
-      <selection activeCell="E26" sqref="E26"/>
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{7D13FC9B-B344-4E74-B7B7-44B6EA59DFDB}">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
     <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}">
       <selection activeCell="E26" sqref="E26"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{7D13FC9B-B344-4E74-B7B7-44B6EA59DFDB}">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
+    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
+      <selection activeCell="E26" sqref="E26"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>

</xml_diff>